<commit_message>
Upadate equetorial guinea form.
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
+++ b/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dyesse\ShareFile\Dossiers personnels\ESPEN\Guinnée Equatorial\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\OEM\Eq Guinea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066154A9-8CC4-4E63-A075-24296632D1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE70741-06D4-4AD0-B6DA-0CA2E0C7C730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -128,9 +128,6 @@
     <t>p_number</t>
   </si>
   <si>
-    <t>p_birth_date</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.3. Fecha nacimiento </t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>En menores de 15 años que contesten los padres</t>
   </si>
   <si>
@@ -365,9 +359,6 @@
     <t>Gota gruesa</t>
   </si>
   <si>
-    <t>select_one samples</t>
-  </si>
-  <si>
     <t>appearance</t>
   </si>
   <si>
@@ -408,6 +399,66 @@
   </si>
   <si>
     <t>1.13.2. En caso afirmativo, la última vez que tuvo esta situación, ¿cuánto tiempo estuvo el gusano antes de desaparecer (en días)?</t>
+  </si>
+  <si>
+    <t>select_multiple samples</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>p_bd_yrs</t>
+  </si>
+  <si>
+    <t>p_bd_months</t>
+  </si>
+  <si>
+    <t>p_bd_day</t>
+  </si>
+  <si>
+    <t>birth_data</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>1.3.1. Año de nacimiento</t>
+  </si>
+  <si>
+    <t>1.3.2. Mes de nacimiento</t>
+  </si>
+  <si>
+    <t>1.3.3. Día de nacimiento</t>
+  </si>
+  <si>
+    <t>El año es incorrecto</t>
+  </si>
+  <si>
+    <t>${p_bd_months} &lt;= 12 and ${p_bd_months} &gt; 0</t>
+  </si>
+  <si>
+    <t>${p_bd_day} &gt; 0 and ${p_bd_day} &lt;= 31</t>
+  </si>
+  <si>
+    <t>${p_bd_yrs} &gt; 1900 and ${p_bd_yrs} &lt; 2005</t>
+  </si>
+  <si>
+    <t>Papel.whatman</t>
+  </si>
+  <si>
+    <t>Gota.gruesa</t>
+  </si>
+  <si>
+    <t>El mes es incorrecto</t>
+  </si>
+  <si>
+    <t>Los días son incorrectos</t>
   </si>
 </sst>
 </file>
@@ -820,21 +871,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.41015625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.8203125" customWidth="1"/>
     <col min="4" max="5" width="20.1171875" customWidth="1"/>
-    <col min="6" max="6" width="18.46875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.46875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.05859375" customWidth="1"/>
     <col min="8" max="8" width="18.46875" customWidth="1"/>
     <col min="9" max="9" width="9.76171875" bestFit="1" customWidth="1"/>
@@ -854,7 +905,7 @@
         <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -869,12 +920,12 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>26</v>
@@ -910,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
@@ -934,7 +985,7 @@
     </row>
     <row r="5" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>32</v>
@@ -953,13 +1004,13 @@
     </row>
     <row r="6" spans="1:10" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>7</v>
@@ -967,40 +1018,39 @@
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
@@ -1009,18 +1059,22 @@
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="5" t="s">
         <v>7</v>
@@ -1028,18 +1082,22 @@
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="5" t="s">
         <v>7</v>
@@ -1047,53 +1105,48 @@
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="F12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1106,74 +1159,72 @@
     </row>
     <row r="14" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="I16" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1186,93 +1237,93 @@
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="I18" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="I19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="H20" s="6"/>
       <c r="I20" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>126</v>
+        <v>43</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="H21" s="6"/>
       <c r="I21" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1285,21 +1336,101 @@
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
+      <c r="I23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1311,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1338,79 +1469,79 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
@@ -1418,13 +1549,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
@@ -1432,13 +1563,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
@@ -1446,13 +1577,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
@@ -1460,13 +1591,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
@@ -1474,13 +1605,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
@@ -1488,13 +1619,13 @@
         <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -1502,13 +1633,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
@@ -1516,13 +1647,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
@@ -1530,13 +1661,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
@@ -1544,13 +1675,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
@@ -1558,13 +1689,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
@@ -1572,13 +1703,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
@@ -1586,13 +1717,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
@@ -1600,13 +1731,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
@@ -1614,13 +1745,13 @@
         <v>15</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
@@ -1628,13 +1759,13 @@
         <v>15</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
@@ -1642,13 +1773,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
@@ -1656,13 +1787,13 @@
         <v>15</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
@@ -1670,10 +1801,10 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
@@ -1681,109 +1812,109 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1822,10 +1953,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C2">
         <v>20191218</v>

</xml_diff>

<commit_message>
Fixed an issue on participant form of OEM Eq. Guinea
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
+++ b/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\OEM\Eq Guinea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE70741-06D4-4AD0-B6DA-0CA2E0C7C730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39FA3DF-8F54-4FEB-9E16-868EBD6DB05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,9 +446,6 @@
     <t>${p_bd_day} &gt; 0 and ${p_bd_day} &lt;= 31</t>
   </si>
   <si>
-    <t>${p_bd_yrs} &gt; 1900 and ${p_bd_yrs} &lt; 2005</t>
-  </si>
-  <si>
     <t>Papel.whatman</t>
   </si>
   <si>
@@ -459,6 +456,9 @@
   </si>
   <si>
     <t>Los días son incorrectos</t>
+  </si>
+  <si>
+    <t>${p_bd_yrs} &gt; 1900 and ${p_bd_yrs} &lt; 2014</t>
   </si>
 </sst>
 </file>
@@ -876,7 +876,7 @@
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1047,7 +1047,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>136</v>
@@ -1073,7 +1073,7 @@
         <v>137</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="5" t="s">
@@ -1096,7 +1096,7 @@
         <v>138</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="5" t="s">
@@ -1900,7 +1900,7 @@
         <v>107</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>108</v>
@@ -1911,7 +1911,7 @@
         <v>107</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Fiw issue on Eq. Guinea form.
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
+++ b/ONCHO/OEM/Eq Guinea/2._OEM_Participant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\OEM\Eq Guinea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39FA3DF-8F54-4FEB-9E16-868EBD6DB05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB6D935-D224-4AAA-BA81-BB60F7876880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,9 +377,6 @@
     <t>select_one SiNo</t>
   </si>
   <si>
-    <t>. &gt;= 15 and .&lt; 135</t>
-  </si>
-  <si>
     <t>${p_had_photo_situation} = "Si"</t>
   </si>
   <si>
@@ -459,6 +456,9 @@
   </si>
   <si>
     <t>${p_bd_yrs} &gt; 1900 and ${p_bd_yrs} &lt; 2014</t>
+  </si>
+  <si>
+    <t>. &gt;= 5 and .&lt; 135</t>
   </si>
 </sst>
 </file>
@@ -876,7 +876,7 @@
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1004,13 +1004,13 @@
     </row>
     <row r="6" spans="1:10" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>7</v>
@@ -1018,17 +1018,17 @@
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1036,21 +1036,21 @@
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
@@ -1059,21 +1059,21 @@
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="5" t="s">
@@ -1082,21 +1082,21 @@
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="5" t="s">
@@ -1105,7 +1105,7 @@
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1128,7 +1128,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>83</v>
@@ -1361,14 +1361,14 @@
         <v>106</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>7</v>
@@ -1382,14 +1382,14 @@
         <v>49</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>7</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>51</v>
@@ -1900,7 +1900,7 @@
         <v>107</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>108</v>
@@ -1911,7 +1911,7 @@
         <v>107</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>109</v>

</xml_diff>